<commit_message>
correctif description (#289) 3a0d2e551dde61ac036d06989314d42956b9c4fe
</commit_message>
<xml_diff>
--- a/ig/main/CodeSystem-ror-include-associated-data-code-system.xlsx
+++ b/ig/main/CodeSystem-ror-include-associated-data-code-system.xlsx
@@ -42,7 +42,7 @@
     <t>Title</t>
   </si>
   <si>
-    <t>Définition des type de phase de l'essai cliniques incluant https://hl7.org/fhir/R4/valueset-research-study-phase.html</t>
+    <t xml:space="preserve">Code System afin d'étendre le Code System pour query parameter includeAssociatedData </t>
   </si>
   <si>
     <t>Status</t>
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-01-15T15:32:20+00:00</t>
+    <t>2024-01-15T15:38:25+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -81,7 +81,7 @@
     <t>Description</t>
   </si>
   <si>
-    <t>type de phase de l'essai clinique</t>
+    <t>Code system pour étendre https://hl7.org/fhir/uv/bulkdata/CodeSystem-include-associated-data.html pour ajouter l'opération export pour le ROR</t>
   </si>
   <si>
     <t>Purpose</t>

</xml_diff>